<commit_message>
Fix: refPeriod 050306TP cube
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-05-050306-A-TP.xlsx
+++ b/data/metadata/Informe-05-050306-A-TP.xlsx
@@ -280,8 +280,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3:M5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,7 +409,7 @@
         <v>34</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,7 +450,7 @@
         <v>35</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,7 +491,7 @@
         <v>38</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>